<commit_message>
updates to eu files to match new us structure
</commit_message>
<xml_diff>
--- a/InputData/trans/BNoGP/BAU Number of Gas Pumps.xlsx
+++ b/InputData/trans/BNoGP/BAU Number of Gas Pumps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\Vensim files from GitHub\EPS EU\InputData\trans\BNoGP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-eu\InputData\trans\BNoGP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331EE0ED-8698-40DB-B7E7-6F753B9A0667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8786C84A-B0FD-4D6D-BB29-4F3F5CB629F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="1305" windowWidth="23430" windowHeight="15060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -108,14 +108,17 @@
     <t>total</t>
   </si>
   <si>
-    <t>BAU EV Chargers</t>
+    <t>BAU Gas Pumps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +164,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -194,12 +204,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -216,8 +227,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="2" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3 2" xfId="1" xr:uid="{3F0B3957-5839-491A-BB84-14323CF38870}"/>
@@ -502,18 +515,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="31.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -521,42 +534,42 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="5">
         <v>2021</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -575,39 +588,39 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
@@ -633,7 +646,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
@@ -659,7 +672,7 @@
         <v>258.5</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>15</v>
       </c>
@@ -685,7 +698,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>20</v>
       </c>
@@ -711,7 +724,7 @@
         <v>420.5</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -721,7 +734,7 @@
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -819,7 +832,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -917,7 +930,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1015,7 +1028,7 @@
         <v>77548</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -1048,185 +1061,185 @@
       <c r="AD17" s="7"/>
       <c r="AE17" s="7"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="7"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="7"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="7"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="7"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="7"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="7"/>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="7"/>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="7"/>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="7"/>
       <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="7"/>
       <c r="H30" s="7"/>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="7"/>
       <c r="H31" s="7"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="7"/>
       <c r="H32" s="7"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="7"/>
       <c r="H33" s="7"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="7"/>
       <c r="H34" s="7"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="7"/>
       <c r="H35" s="7"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="7"/>
       <c r="H36" s="7"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="7"/>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="7"/>
       <c r="H38" s="7"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="7"/>
       <c r="H39" s="7"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="7"/>
       <c r="H40" s="7"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="7"/>
       <c r="H41" s="7"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="7"/>
       <c r="H42" s="7"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="7"/>
       <c r="H43" s="7"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="7"/>
       <c r="H44" s="7"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="7"/>
       <c r="H45" s="7"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="7"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="7"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="7"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="7"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="7"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="7"/>
@@ -1247,12 +1260,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1347,11 +1360,11 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="12">
         <f>Calculations!C14*10</f>
         <v>1362850</v>
       </c>
@@ -1479,6 +1492,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="14" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="4a12692b057bc30d68596ac87c75a308">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4dd464ebbb7361a2027b4bc4be8d527a" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -1707,27 +1740,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58EF8824-9526-4355-8C1F-9528CCE4920E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9D480BD-2350-4E3F-8A60-31F7B799F325}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94825B5B-5551-428A-ACDB-9F3C83C6C691}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1744,23 +1776,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9D480BD-2350-4E3F-8A60-31F7B799F325}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58EF8824-9526-4355-8C1F-9528CCE4920E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>